<commit_message>
adding a bunch of functions and the monitoring script
</commit_message>
<xml_diff>
--- a/calibration_files/68179/68179.xlsx
+++ b/calibration_files/68179/68179.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f58868ea66379a41/Documents/GitHub/orpheus_magnet_test/calibration_files/68179/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{55C1827F-2A22-4828-B8A1-A0C17E94C41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36877E9D-EA59-4782-B7A7-FC1C785C9485}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{55C1827F-2A22-4828-B8A1-A0C17E94C41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{545B26B4-23C7-4840-B282-5BDF2FCF9015}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A233C0FE-35EB-4EF3-99FD-2DED87E99418}"/>
   </bookViews>
@@ -2569,7 +2569,7 @@
   <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2608,6 +2608,10 @@
         <f t="shared" ref="C3:C66" si="0">A3/1000</f>
         <v>-2.3934840000000002E-2</v>
       </c>
+      <c r="E3" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,C2:C66)</f>
+        <v>-0.02475739,-0.02393484,-0.02311216,-0.02228932,-0.02146634,-0.02064321,-0.01981993,-0.01899651,-0.01817295,-0.01734923,-0.01652538,-0.01570139,-0.01487725,-0.01405296,-0.01322854,-0.01240399,-0.01157926,-0.01075431,-0.00992915,-0.00910377,-0.00827804,-0.00745186,-0.0066253,-0.00579832,-0.00497093,-0.00414316,-0.00331502,-0.00248652,-0.00165777,-0.00082897,-0.0002487,-0.00004145,0,0.00004144,0.00024866,0.00082882,0.00165765,0.00248596,0.00331392,0.00414162,0.00496892,0.00579558,0.00662184,0.0074478,0.00827331,0.00909826,0.00992278,0.01074718,0.01157142,0.01239546,0.01321935,0.01404313,0.01486683,0.01569045,0.01651398,0.01733738,0.01816066,0.01898384,0.01980691,0.02062986,0.02145271,0.02227545,0.02309808,0.0239206,0.02474302</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -3375,6 +3379,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added calibrations and functions for three additional hall sensors
</commit_message>
<xml_diff>
--- a/calibration_files/68179/68179.xlsx
+++ b/calibration_files/68179/68179.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f58868ea66379a41/Documents/GitHub/orpheus_magnet_test/calibration_files/68179/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{55C1827F-2A22-4828-B8A1-A0C17E94C41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{545B26B4-23C7-4840-B282-5BDF2FCF9015}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{55C1827F-2A22-4828-B8A1-A0C17E94C41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FE91383-2913-42F8-AAB0-85030550397B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A233C0FE-35EB-4EF3-99FD-2DED87E99418}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2245,8 +2248,26 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="D1" t="str">
+            <v>-0.02533235,-0.02450252,-0.02367162,-0.02283963,-0.02200657,-0.02117245,-0.02033726,-0.01950101,-0.01866371,-0.01782536,-0.01698597,-0.01614554,-0.01530407,-0.01446156,-0.01361804,-0.01277349,-0.01192973,-0.01108135,-0.01023376,-0.00938518,-0.00853555,-0.0076848,-0.00683338,-0.0059802,-0.00512614,-0.00427265,-0.00341867,-0.00256472,-0.00171049,-0.00085587,-0.00025757,-0.00004397,0,0.00004363,0.00025525,0.00085264,0.0017059,0.00255888,0.00341129,0.00426294,0.00511377,0.00596421,0.0068132,0.00766109,0.00850901,0.00935618,0.01020277,0.01104884,0.01189438,0.01273939,0.01358385,0.01442775,0.01527108,0.01611383,0.01695598,0.01779754,0.01863847,0.01947879,0.02031846,0.02115749,0.02199586,0.02283356,0.02367058,0.02450691,0.02534253</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2609,8 +2630,8 @@
         <v>-2.3934840000000002E-2</v>
       </c>
       <c r="E3" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,C2:C66)</f>
-        <v>-0.02475739,-0.02393484,-0.02311216,-0.02228932,-0.02146634,-0.02064321,-0.01981993,-0.01899651,-0.01817295,-0.01734923,-0.01652538,-0.01570139,-0.01487725,-0.01405296,-0.01322854,-0.01240399,-0.01157926,-0.01075431,-0.00992915,-0.00910377,-0.00827804,-0.00745186,-0.0066253,-0.00579832,-0.00497093,-0.00414316,-0.00331502,-0.00248652,-0.00165777,-0.00082897,-0.0002487,-0.00004145,0,0.00004144,0.00024866,0.00082882,0.00165765,0.00248596,0.00331392,0.00414162,0.00496892,0.00579558,0.00662184,0.0074478,0.00827331,0.00909826,0.00992278,0.01074718,0.01157142,0.01239546,0.01321935,0.01404313,0.01486683,0.01569045,0.01651398,0.01733738,0.01816066,0.01898384,0.01980691,0.02062986,0.02145271,0.02227545,0.02309808,0.0239206,0.02474302</v>
+        <f>[1]Sheet1!$D$1</f>
+        <v>-0.02533235,-0.02450252,-0.02367162,-0.02283963,-0.02200657,-0.02117245,-0.02033726,-0.01950101,-0.01866371,-0.01782536,-0.01698597,-0.01614554,-0.01530407,-0.01446156,-0.01361804,-0.01277349,-0.01192973,-0.01108135,-0.01023376,-0.00938518,-0.00853555,-0.0076848,-0.00683338,-0.0059802,-0.00512614,-0.00427265,-0.00341867,-0.00256472,-0.00171049,-0.00085587,-0.00025757,-0.00004397,0,0.00004363,0.00025525,0.00085264,0.0017059,0.00255888,0.00341129,0.00426294,0.00511377,0.00596421,0.0068132,0.00766109,0.00850901,0.00935618,0.01020277,0.01104884,0.01189438,0.01273939,0.01358385,0.01442775,0.01527108,0.01611383,0.01695598,0.01779754,0.01863847,0.01947879,0.02031846,0.02115749,0.02199586,0.02283356,0.02367058,0.02450691,0.02534253</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>